<commit_message>
Added Green Outline when selected Added Department Change Functionality Corrected Left Right images Added WTA calculation
</commit_message>
<xml_diff>
--- a/Final Capstone/GUI/build/assets/DB/Configuration.xlsx
+++ b/Final Capstone/GUI/build/assets/DB/Configuration.xlsx
@@ -5,73 +5,63 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weiji\PycharmProjects\MtechISS\Final Capstone\GUI\build\assets\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\PycharmProjects\MtechISS\Final Capstone\GUI\build\assets\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF0B0E3-3E6E-42AF-B59C-C253DF40E733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6C81A2-E869-4E21-9079-0BBAC3F103DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Configuration!$A$1:$I$38</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Config Key</t>
+  </si>
+  <si>
+    <t>Config Value</t>
+  </si>
+  <si>
+    <t>DB_FILE</t>
+  </si>
   <si>
     <t>./assets/DB/DB File.xlsx</t>
   </si>
   <si>
+    <t>DB_CONFIG</t>
+  </si>
+  <si>
     <t>./assets/DB/Department Short Codes.xlsx</t>
   </si>
   <si>
-    <t>DB_CONFIG</t>
-  </si>
-  <si>
-    <t>DB_FILE</t>
-  </si>
-  <si>
-    <t>Config Key</t>
-  </si>
-  <si>
-    <t>Config Value</t>
+    <t>SECONDARY_COLOR</t>
   </si>
   <si>
     <t>#030C5D</t>
   </si>
   <si>
+    <t>BACKGROUND_COLOR</t>
+  </si>
+  <si>
     <t>#EDFFF6</t>
   </si>
   <si>
+    <t>BTN_COLOR</t>
+  </si>
+  <si>
     <t>#007D3E</t>
   </si>
   <si>
-    <t>SECONDARY_COLOR</t>
-  </si>
-  <si>
-    <t>BACKGROUND_COLOR</t>
-  </si>
-  <si>
-    <t>BTN_COLOR</t>
+    <t>DEFAULT_SEARCH_FOLDER</t>
+  </si>
+  <si>
+    <t>C:/Users/USER/National University of Singapore/MTech Y1S2 - Documents/General/Final Capstone Project/Dataset</t>
   </si>
 </sst>
 </file>
@@ -103,10 +93,36 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -115,9 +131,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,72 +416,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="34.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1328125" customWidth="1"/>
-    <col min="7" max="7" width="22.86328125" customWidth="1"/>
-    <col min="8" max="8" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>